<commit_message>
add jordan fp Rmd
</commit_message>
<xml_diff>
--- a/data/Paul/comp_var_Paul_thesis_vs_TAMASA.xlsx
+++ b/data/Paul/comp_var_Paul_thesis_vs_TAMASA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TAMASA\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TAMASA\data\Paul\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA692F63-86B1-4BA9-AB50-E467870CF4E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DF265C56-A9B2-442C-93D5-C594D1CBF63B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="7875" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="7875" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_local_currency" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,11 @@
     <sheet name="labour_day8h" sheetId="4" r:id="rId4"/>
     <sheet name="Linking cost variables TAMASA" sheetId="7" r:id="rId5"/>
     <sheet name="linking labour variables TAMASA" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Sheet1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
@@ -423,8 +427,93 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>appravensbergen</author>
+  </authors>
+  <commentList>
+    <comment ref="A10" authorId="0" shapeId="0" xr:uid="{E6C519FA-4149-4D2C-832C-DAB7BACF016E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>appravensbergen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Rachier 2005, Maingi 2001, CAN 27 % N</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A11" authorId="0" shapeId="0" xr:uid="{1DE98B5C-A7D4-4D97-9DAF-02BED6524CFC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>appravensbergen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Tamado 2007, Alemayehu, 2017 18%N, 20%P
+Rusinamhodzi 2017, 18%N, 46%P2O5
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{9B88B645-92AD-4924-A3EB-8902DCE80A2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>appravensbergen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+also adds 0.90 kg of N
+ </t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="132">
   <si>
     <t>Country</t>
   </si>
@@ -713,6 +802,114 @@
   <si>
     <t xml:space="preserve">no data </t>
   </si>
+  <si>
+    <t>From TAMASA</t>
+  </si>
+  <si>
+    <t>From Expert</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>price local maize seed (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price hybrid maize seed (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price local pigeon pea seeds (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price improved pigeon pea seeds (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price CAN (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price DAP (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price N (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price P (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price NPK (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price TSP (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>refer to as pesticide</t>
+  </si>
+  <si>
+    <t>price insecticide (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>price fungicide  (Tsh/L)</t>
+  </si>
+  <si>
+    <t>price herbicide  (Tsh/L)</t>
+  </si>
+  <si>
+    <t>to few data points</t>
+  </si>
+  <si>
+    <t>selling price maize (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>selling price pigeon pea  (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>sowing (day/ha)</t>
+  </si>
+  <si>
+    <t>refer to as planting</t>
+  </si>
+  <si>
+    <t>fertilizer application (day/ha)</t>
+  </si>
+  <si>
+    <t>herbicide application (day/ha)</t>
+  </si>
+  <si>
+    <t>weeding (day/ha)</t>
+  </si>
+  <si>
+    <t>harvesting maize (day/ton)</t>
+  </si>
+  <si>
+    <t>harvesting legume (day/ton)</t>
+  </si>
+  <si>
+    <t>harvesting (day/ton)</t>
+  </si>
+  <si>
+    <t>treshing maize (day/ton)</t>
+  </si>
+  <si>
+    <t>treshing legume (day/ton)</t>
+  </si>
+  <si>
+    <t>treshing (day/ha)</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>price urea (Tsh/kg)</t>
+  </si>
+  <si>
+    <t>land preparation (day/ha)</t>
+  </si>
+  <si>
+    <t>problem</t>
+  </si>
 </sst>
 </file>
 
@@ -721,7 +918,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,8 +986,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -805,6 +1009,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1117,7 +1326,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -1133,8 +1342,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1176,8 +1386,10 @@
       <alignment textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="11" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
+    <cellStyle name="Bad" xfId="11" builtinId="27"/>
     <cellStyle name="Calculation" xfId="10" builtinId="22"/>
     <cellStyle name="Input" xfId="8" builtinId="20"/>
     <cellStyle name="Module title" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -4977,8 +5189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D06573A-A8F5-4AAD-B0B3-6E8108579E0D}">
   <dimension ref="A1:D16380"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5203,10 +5415,10 @@
         <v>63</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -54300,7 +54512,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54429,22 +54641,465 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B44BDF5-A905-485D-A02D-1DA3606DD18E}">
+  <dimension ref="A1:F31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="37" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="D15" s="3">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="36" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31">
+        <f>SUM(B2:B28)</f>
+        <v>20</v>
+      </c>
+      <c r="D31">
+        <f>SUM(D2:D28)</f>
+        <v>7</v>
+      </c>
+      <c r="E31">
+        <f>SUM(B31:D31)</f>
+        <v>27</v>
+      </c>
+      <c r="F31">
+        <f>SUM(F2:F28)</f>
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1" xr:uid="{7159C04E-BAEB-443E-BD64-F63C6BD64B9E}">
+    <sortState ref="A2:F28">
+      <sortCondition descending="1" ref="F1"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:F28">
+    <sortCondition ref="A2"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009810AB5F2911E64683BAEC42E7B886E6" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="ca1fbb159048343a84ed76b6e4d91d8d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42935c7d-9f47-4399-b135-59bc620e0da9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d462d4cd21746c9dd51fafdfa118bae1" ns3:_="">
     <xsd:import namespace="42935c7d-9f47-4399-b135-59bc620e0da9"/>
@@ -54614,31 +55269,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BFD4D3D-3296-4263-B14C-5DD7535BCB14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="42935c7d-9f47-4399-b135-59bc620e0da9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E711286-A16B-44D6-85BE-61591783C649}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B921580B-FE11-49B1-BAD4-9EA660F15EBD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54654,4 +55300,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E711286-A16B-44D6-85BE-61591783C649}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BFD4D3D-3296-4263-B14C-5DD7535BCB14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="42935c7d-9f47-4399-b135-59bc620e0da9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>